<commit_message>
changes to spec to make it easier to write code with its data, tested two objectives
</commit_message>
<xml_diff>
--- a/draft.xlsx
+++ b/draft.xlsx
@@ -13,6 +13,8 @@
     <sheet name="plan_taskConfig" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="plan_datesConfig" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="people" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="people_parameters" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="peopleRelations" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t xml:space="preserve">taskName</t>
   </si>
@@ -59,6 +61,24 @@
     <t xml:space="preserve">endDate</t>
   </si>
   <si>
+    <t xml:space="preserve">holiday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preholiday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prepreholiday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prethreeday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">special</t>
+  </si>
+  <si>
+    <t xml:space="preserve">threeday</t>
+  </si>
+  <si>
     <t xml:space="preserve">defaultCount</t>
   </si>
   <si>
@@ -135,6 +155,30 @@
   </si>
   <si>
     <t xml:space="preserve">parameters/minimumGap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">john</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOHN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peopleRelations</t>
   </si>
 </sst>
 </file>
@@ -217,7 +261,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -238,6 +282,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -246,8 +294,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -464,15 +516,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:XFD2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.94"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -482,12 +540,31 @@
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="XFD1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
+      <c r="A2" s="6" t="n">
         <v>45261</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="6" t="n">
         <v>45291</v>
       </c>
     </row>
@@ -526,13 +603,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -588,28 +665,28 @@
         <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -632,10 +709,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -658,54 +735,666 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="22.84"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="6" t="s">
+    <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="B1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="H1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AH53"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="4" style="0" width="10.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="15" style="0" width="10.63"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>36</v>
+      <c r="D1" s="9" t="n">
+        <v>45261</v>
+      </c>
+      <c r="E1" s="9" t="n">
+        <v>45262</v>
+      </c>
+      <c r="F1" s="9" t="n">
+        <v>45263</v>
+      </c>
+      <c r="G1" s="9" t="n">
+        <v>45264</v>
+      </c>
+      <c r="H1" s="9" t="n">
+        <v>45265</v>
+      </c>
+      <c r="I1" s="9" t="n">
+        <v>45266</v>
+      </c>
+      <c r="J1" s="9" t="n">
+        <v>45267</v>
+      </c>
+      <c r="K1" s="9" t="n">
+        <v>45268</v>
+      </c>
+      <c r="L1" s="9" t="n">
+        <v>45269</v>
+      </c>
+      <c r="M1" s="9" t="n">
+        <v>45270</v>
+      </c>
+      <c r="N1" s="9" t="n">
+        <v>45271</v>
+      </c>
+      <c r="O1" s="9" t="n">
+        <v>45272</v>
+      </c>
+      <c r="P1" s="9" t="n">
+        <v>45273</v>
+      </c>
+      <c r="Q1" s="9" t="n">
+        <v>45274</v>
+      </c>
+      <c r="R1" s="9" t="n">
+        <v>45275</v>
+      </c>
+      <c r="S1" s="9" t="n">
+        <v>45276</v>
+      </c>
+      <c r="T1" s="9" t="n">
+        <v>45277</v>
+      </c>
+      <c r="U1" s="9" t="n">
+        <v>45278</v>
+      </c>
+      <c r="V1" s="9" t="n">
+        <v>45279</v>
+      </c>
+      <c r="W1" s="9" t="n">
+        <v>45280</v>
+      </c>
+      <c r="X1" s="9" t="n">
+        <v>45281</v>
+      </c>
+      <c r="Y1" s="9" t="n">
+        <v>45282</v>
+      </c>
+      <c r="Z1" s="9" t="n">
+        <v>45283</v>
+      </c>
+      <c r="AA1" s="9" t="n">
+        <v>45284</v>
+      </c>
+      <c r="AB1" s="9" t="n">
+        <v>45285</v>
+      </c>
+      <c r="AC1" s="9" t="n">
+        <v>45286</v>
+      </c>
+      <c r="AD1" s="9" t="n">
+        <v>45287</v>
+      </c>
+      <c r="AE1" s="9" t="n">
+        <v>45288</v>
+      </c>
+      <c r="AF1" s="9" t="n">
+        <v>45289</v>
+      </c>
+      <c r="AG1" s="9" t="n">
+        <v>45290</v>
+      </c>
+      <c r="AH1" s="9" t="n">
+        <v>45291</v>
+      </c>
+    </row>
+    <row r="2" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
+    </row>
+    <row r="3" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A52"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K29" activeCellId="0" sqref="K29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="15.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="8" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="str">
+        <f aca="false">people!A2&amp;" "&amp;people!B2&amp;" "&amp;people!C2</f>
+        <v>john lol </v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="str">
+        <f aca="false">people!A3&amp;" "&amp;people!B3&amp;" "&amp;people!C3</f>
+        <v>mar lith </v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="str">
+        <f aca="false">people!A4&amp;" "&amp;people!B4&amp;" "&amp;people!C4</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="str">
+        <f aca="false">people!A5&amp;" "&amp;people!B5&amp;" "&amp;people!C5</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="str">
+        <f aca="false">people!A6&amp;" "&amp;people!B6&amp;" "&amp;people!C6</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="str">
+        <f aca="false">people!A7&amp;" "&amp;people!B7&amp;" "&amp;people!C7</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="str">
+        <f aca="false">people!A8&amp;" "&amp;people!B8&amp;" "&amp;people!C8</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="str">
+        <f aca="false">people!A9&amp;" "&amp;people!B9&amp;" "&amp;people!C9</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="str">
+        <f aca="false">people!A10&amp;" "&amp;people!B10&amp;" "&amp;people!C10</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="str">
+        <f aca="false">people!A11&amp;" "&amp;people!B11&amp;" "&amp;people!C11</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="str">
+        <f aca="false">people!A12&amp;" "&amp;people!B12&amp;" "&amp;people!C12</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="str">
+        <f aca="false">people!A13&amp;" "&amp;people!B13&amp;" "&amp;people!C13</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="str">
+        <f aca="false">people!A14&amp;" "&amp;people!B14&amp;" "&amp;people!C14</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="str">
+        <f aca="false">people!A15&amp;" "&amp;people!B15&amp;" "&amp;people!C15</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="str">
+        <f aca="false">people!A16&amp;" "&amp;people!B16&amp;" "&amp;people!C16</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="str">
+        <f aca="false">people!A17&amp;" "&amp;people!B17&amp;" "&amp;people!C17</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="str">
+        <f aca="false">people!A18&amp;" "&amp;people!B18&amp;" "&amp;people!C18</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="str">
+        <f aca="false">people!A19&amp;" "&amp;people!B19&amp;" "&amp;people!C19</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="str">
+        <f aca="false">people!A20&amp;" "&amp;people!B20&amp;" "&amp;people!C20</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="str">
+        <f aca="false">people!A21&amp;" "&amp;people!B21&amp;" "&amp;people!C21</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="str">
+        <f aca="false">people!A22&amp;" "&amp;people!B22&amp;" "&amp;people!C22</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="str">
+        <f aca="false">people!A23&amp;" "&amp;people!B23&amp;" "&amp;people!C23</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="str">
+        <f aca="false">people!A24&amp;" "&amp;people!B24&amp;" "&amp;people!C24</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="str">
+        <f aca="false">people!A25&amp;" "&amp;people!B25&amp;" "&amp;people!C25</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="str">
+        <f aca="false">people!A26&amp;" "&amp;people!B26&amp;" "&amp;people!C26</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="str">
+        <f aca="false">people!A27&amp;" "&amp;people!B27&amp;" "&amp;people!C27</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="str">
+        <f aca="false">people!A28&amp;" "&amp;people!B28&amp;" "&amp;people!C28</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="str">
+        <f aca="false">people!A29&amp;" "&amp;people!B29&amp;" "&amp;people!C29</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="str">
+        <f aca="false">people!A30&amp;" "&amp;people!B30&amp;" "&amp;people!C30</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="str">
+        <f aca="false">people!A31&amp;" "&amp;people!B31&amp;" "&amp;people!C31</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="8" t="str">
+        <f aca="false">people!A32&amp;" "&amp;people!B32&amp;" "&amp;people!C32</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="str">
+        <f aca="false">people!A33&amp;" "&amp;people!B33&amp;" "&amp;people!C33</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="str">
+        <f aca="false">people!A34&amp;" "&amp;people!B34&amp;" "&amp;people!C34</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="8" t="str">
+        <f aca="false">people!A35&amp;" "&amp;people!B35&amp;" "&amp;people!C35</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="8" t="str">
+        <f aca="false">people!A36&amp;" "&amp;people!B36&amp;" "&amp;people!C36</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="8" t="str">
+        <f aca="false">people!A37&amp;" "&amp;people!B37&amp;" "&amp;people!C37</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="8" t="str">
+        <f aca="false">people!A38&amp;" "&amp;people!B38&amp;" "&amp;people!C38</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="8" t="str">
+        <f aca="false">people!A39&amp;" "&amp;people!B39&amp;" "&amp;people!C39</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8" t="str">
+        <f aca="false">people!A40&amp;" "&amp;people!B40&amp;" "&amp;people!C40</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="8" t="str">
+        <f aca="false">people!A41&amp;" "&amp;people!B41&amp;" "&amp;people!C41</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="8" t="str">
+        <f aca="false">people!A42&amp;" "&amp;people!B42&amp;" "&amp;people!C42</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="8" t="str">
+        <f aca="false">people!A43&amp;" "&amp;people!B43&amp;" "&amp;people!C43</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="8" t="str">
+        <f aca="false">people!A44&amp;" "&amp;people!B44&amp;" "&amp;people!C44</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="8" t="str">
+        <f aca="false">people!A45&amp;" "&amp;people!B45&amp;" "&amp;people!C45</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="8" t="str">
+        <f aca="false">people!A46&amp;" "&amp;people!B46&amp;" "&amp;people!C46</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="8" t="str">
+        <f aca="false">people!A47&amp;" "&amp;people!B47&amp;" "&amp;people!C47</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="8" t="str">
+        <f aca="false">people!A48&amp;" "&amp;people!B48&amp;" "&amp;people!C48</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="8" t="str">
+        <f aca="false">people!A49&amp;" "&amp;people!B49&amp;" "&amp;people!C49</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="8" t="str">
+        <f aca="false">people!A50&amp;" "&amp;people!B50&amp;" "&amp;people!C50</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="8" t="str">
+        <f aca="false">people!A51&amp;" "&amp;people!B51&amp;" "&amp;people!C51</f>
+        <v>  </v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="8" t="str">
+        <f aca="false">people!A52&amp;" "&amp;people!B52&amp;" "&amp;people!C52</f>
+        <v>  </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make able to work with both json and xlsx as draft input
</commit_message>
<xml_diff>
--- a/draft.xlsx
+++ b/draft.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="1" state="visible" r:id="rId3"/>
@@ -13,7 +13,7 @@
     <sheet name="plan_taskConfig" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="plan_datesConfig" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="people" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="people_parameters" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="preferences" sheetId="6" state="visible" r:id="rId8"/>
     <sheet name="peopleRelations" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="83">
   <si>
     <t xml:space="preserve">taskName</t>
   </si>
@@ -79,6 +79,12 @@
     <t xml:space="preserve">threeday</t>
   </si>
   <si>
+    <t xml:space="preserve">2023-12-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-31</t>
+  </si>
+  <si>
     <t xml:space="preserve">defaultCount</t>
   </si>
   <si>
@@ -115,7 +121,7 @@
     <t xml:space="preserve">lastName</t>
   </si>
   <si>
-    <t xml:space="preserve">fatherName</t>
+    <t xml:space="preserve">uuid</t>
   </si>
   <si>
     <t xml:space="preserve">rank/rankName</t>
@@ -163,19 +169,109 @@
     <t xml:space="preserve">lol</t>
   </si>
   <si>
+    <t xml:space="preserve">LOLAS</t>
+  </si>
+  <si>
     <t xml:space="preserve">mar</t>
   </si>
   <si>
     <t xml:space="preserve">lith</t>
   </si>
   <si>
-    <t xml:space="preserve">JOHN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IL</t>
+    <t xml:space="preserve">LITHO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not</t>
   </si>
   <si>
     <t xml:space="preserve">peopleRelations</t>
@@ -185,9 +281,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -261,7 +358,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -278,11 +375,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -290,15 +391,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -427,8 +532,8 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -437,7 +542,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -519,54 +624,60 @@
   <dimension ref="A1:XFD2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="K56" activeCellId="0" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.94"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="XFD1" s="0"/>
+      <c r="XFD1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="n">
-        <v>45261</v>
-      </c>
-      <c r="B2" s="6" t="n">
-        <v>45291</v>
-      </c>
+      <c r="A2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -587,15 +698,15 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="12.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="13.93"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -603,13 +714,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -619,8 +730,8 @@
       <c r="B2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -638,7 +749,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
@@ -665,33 +776,29 @@
         <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E2" s="0"/>
-      <c r="F2" s="0"/>
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -711,123 +818,127 @@
   </sheetPr>
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="22.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="22.84"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="7" t="s">
+    <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="F1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="G1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="H1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="I1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="J1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="K1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="L1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="M1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="N1" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="O1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
+      <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
+      <c r="A3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -848,138 +959,147 @@
   <dimension ref="A1:AH53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="4" style="0" width="10.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="15" style="0" width="10.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="10.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="13" style="1" width="10.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="33" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>27</v>
+    <row r="1" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="9" t="n">
-        <v>45261</v>
-      </c>
-      <c r="E1" s="9" t="n">
-        <v>45262</v>
-      </c>
-      <c r="F1" s="9" t="n">
-        <v>45263</v>
-      </c>
-      <c r="G1" s="9" t="n">
-        <v>45264</v>
-      </c>
-      <c r="H1" s="9" t="n">
-        <v>45265</v>
-      </c>
-      <c r="I1" s="9" t="n">
-        <v>45266</v>
-      </c>
-      <c r="J1" s="9" t="n">
-        <v>45267</v>
-      </c>
-      <c r="K1" s="9" t="n">
-        <v>45268</v>
-      </c>
-      <c r="L1" s="9" t="n">
-        <v>45269</v>
-      </c>
-      <c r="M1" s="9" t="n">
-        <v>45270</v>
-      </c>
-      <c r="N1" s="9" t="n">
-        <v>45271</v>
-      </c>
-      <c r="O1" s="9" t="n">
-        <v>45272</v>
-      </c>
-      <c r="P1" s="9" t="n">
-        <v>45273</v>
-      </c>
-      <c r="Q1" s="9" t="n">
-        <v>45274</v>
-      </c>
-      <c r="R1" s="9" t="n">
-        <v>45275</v>
-      </c>
-      <c r="S1" s="9" t="n">
-        <v>45276</v>
-      </c>
-      <c r="T1" s="9" t="n">
-        <v>45277</v>
-      </c>
-      <c r="U1" s="9" t="n">
-        <v>45278</v>
-      </c>
-      <c r="V1" s="9" t="n">
-        <v>45279</v>
-      </c>
-      <c r="W1" s="9" t="n">
-        <v>45280</v>
-      </c>
-      <c r="X1" s="9" t="n">
-        <v>45281</v>
-      </c>
-      <c r="Y1" s="9" t="n">
-        <v>45282</v>
-      </c>
-      <c r="Z1" s="9" t="n">
-        <v>45283</v>
-      </c>
-      <c r="AA1" s="9" t="n">
-        <v>45284</v>
-      </c>
-      <c r="AB1" s="9" t="n">
-        <v>45285</v>
-      </c>
-      <c r="AC1" s="9" t="n">
-        <v>45286</v>
-      </c>
-      <c r="AD1" s="9" t="n">
-        <v>45287</v>
-      </c>
-      <c r="AE1" s="9" t="n">
-        <v>45288</v>
-      </c>
-      <c r="AF1" s="9" t="n">
-        <v>45289</v>
-      </c>
-      <c r="AG1" s="9" t="n">
-        <v>45290</v>
-      </c>
-      <c r="AH1" s="9" t="n">
-        <v>45291</v>
-      </c>
-    </row>
-    <row r="2" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG1" s="7"/>
+      <c r="AH1" s="7"/>
+    </row>
+    <row r="2" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+        <v>80</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -1007,57 +1127,119 @@
       <c r="AG2" s="4"/>
       <c r="AH2" s="4"/>
     </row>
-    <row r="3" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11"/>
+    </row>
+    <row r="5" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11"/>
+    </row>
+    <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11"/>
+    </row>
+    <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11"/>
+    </row>
+    <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11"/>
+    </row>
+    <row r="9" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11"/>
+    </row>
+    <row r="10" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11"/>
+    </row>
+    <row r="11" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11"/>
+    </row>
+    <row r="12" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11"/>
+    </row>
+    <row r="13" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11"/>
+    </row>
+    <row r="14" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11"/>
+    </row>
+    <row r="15" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11"/>
+    </row>
+    <row r="16" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11"/>
+    </row>
+    <row r="17" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11"/>
+    </row>
+    <row r="18" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11"/>
+    </row>
+    <row r="19" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="11"/>
+    </row>
+    <row r="20" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="11"/>
+    </row>
+    <row r="21" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="11"/>
+    </row>
+    <row r="22" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11"/>
+    </row>
+    <row r="23" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="11"/>
+    </row>
+    <row r="24" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="11"/>
+    </row>
+    <row r="25" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="11"/>
+    </row>
+    <row r="26" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="11"/>
+    </row>
+    <row r="27" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="11"/>
+    </row>
+    <row r="28" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="11"/>
+    </row>
+    <row r="29" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="11"/>
+    </row>
+    <row r="30" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="11"/>
+    </row>
+    <row r="31" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="11"/>
+    </row>
+    <row r="32" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="11"/>
+    </row>
+    <row r="33" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1082,317 +1264,317 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="15.27"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="8" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="15.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>50</v>
+      <c r="A1" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="str">
+      <c r="A2" s="3" t="str">
         <f aca="false">people!A2&amp;" "&amp;people!B2&amp;" "&amp;people!C2</f>
-        <v>john lol </v>
+        <v>john lol LOLAS</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="str">
+      <c r="A3" s="3" t="str">
         <f aca="false">people!A3&amp;" "&amp;people!B3&amp;" "&amp;people!C3</f>
-        <v>mar lith </v>
+        <v>mar lith LITHO</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="str">
+      <c r="A4" s="3" t="str">
         <f aca="false">people!A4&amp;" "&amp;people!B4&amp;" "&amp;people!C4</f>
         <v>  </v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="str">
+      <c r="A5" s="3" t="str">
         <f aca="false">people!A5&amp;" "&amp;people!B5&amp;" "&amp;people!C5</f>
         <v>  </v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="str">
+      <c r="A6" s="3" t="str">
         <f aca="false">people!A6&amp;" "&amp;people!B6&amp;" "&amp;people!C6</f>
         <v>  </v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="str">
+      <c r="A7" s="3" t="str">
         <f aca="false">people!A7&amp;" "&amp;people!B7&amp;" "&amp;people!C7</f>
         <v>  </v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="str">
+      <c r="A8" s="3" t="str">
         <f aca="false">people!A8&amp;" "&amp;people!B8&amp;" "&amp;people!C8</f>
         <v>  </v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="str">
+      <c r="A9" s="3" t="str">
         <f aca="false">people!A9&amp;" "&amp;people!B9&amp;" "&amp;people!C9</f>
         <v>  </v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="str">
+      <c r="A10" s="3" t="str">
         <f aca="false">people!A10&amp;" "&amp;people!B10&amp;" "&amp;people!C10</f>
         <v>  </v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="str">
+      <c r="A11" s="3" t="str">
         <f aca="false">people!A11&amp;" "&amp;people!B11&amp;" "&amp;people!C11</f>
         <v>  </v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="str">
+      <c r="A12" s="3" t="str">
         <f aca="false">people!A12&amp;" "&amp;people!B12&amp;" "&amp;people!C12</f>
         <v>  </v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="str">
+      <c r="A13" s="3" t="str">
         <f aca="false">people!A13&amp;" "&amp;people!B13&amp;" "&amp;people!C13</f>
         <v>  </v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="str">
+      <c r="A14" s="3" t="str">
         <f aca="false">people!A14&amp;" "&amp;people!B14&amp;" "&amp;people!C14</f>
         <v>  </v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="str">
+      <c r="A15" s="3" t="str">
         <f aca="false">people!A15&amp;" "&amp;people!B15&amp;" "&amp;people!C15</f>
         <v>  </v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="str">
+      <c r="A16" s="3" t="str">
         <f aca="false">people!A16&amp;" "&amp;people!B16&amp;" "&amp;people!C16</f>
         <v>  </v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="str">
+      <c r="A17" s="3" t="str">
         <f aca="false">people!A17&amp;" "&amp;people!B17&amp;" "&amp;people!C17</f>
         <v>  </v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="str">
+      <c r="A18" s="3" t="str">
         <f aca="false">people!A18&amp;" "&amp;people!B18&amp;" "&amp;people!C18</f>
         <v>  </v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="str">
+      <c r="A19" s="3" t="str">
         <f aca="false">people!A19&amp;" "&amp;people!B19&amp;" "&amp;people!C19</f>
         <v>  </v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="str">
+      <c r="A20" s="3" t="str">
         <f aca="false">people!A20&amp;" "&amp;people!B20&amp;" "&amp;people!C20</f>
         <v>  </v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="str">
+      <c r="A21" s="3" t="str">
         <f aca="false">people!A21&amp;" "&amp;people!B21&amp;" "&amp;people!C21</f>
         <v>  </v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="str">
+      <c r="A22" s="3" t="str">
         <f aca="false">people!A22&amp;" "&amp;people!B22&amp;" "&amp;people!C22</f>
         <v>  </v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="str">
+      <c r="A23" s="3" t="str">
         <f aca="false">people!A23&amp;" "&amp;people!B23&amp;" "&amp;people!C23</f>
         <v>  </v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="str">
+      <c r="A24" s="3" t="str">
         <f aca="false">people!A24&amp;" "&amp;people!B24&amp;" "&amp;people!C24</f>
         <v>  </v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="str">
+      <c r="A25" s="3" t="str">
         <f aca="false">people!A25&amp;" "&amp;people!B25&amp;" "&amp;people!C25</f>
         <v>  </v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="str">
+      <c r="A26" s="3" t="str">
         <f aca="false">people!A26&amp;" "&amp;people!B26&amp;" "&amp;people!C26</f>
         <v>  </v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="str">
+      <c r="A27" s="3" t="str">
         <f aca="false">people!A27&amp;" "&amp;people!B27&amp;" "&amp;people!C27</f>
         <v>  </v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="str">
+      <c r="A28" s="3" t="str">
         <f aca="false">people!A28&amp;" "&amp;people!B28&amp;" "&amp;people!C28</f>
         <v>  </v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="str">
+      <c r="A29" s="3" t="str">
         <f aca="false">people!A29&amp;" "&amp;people!B29&amp;" "&amp;people!C29</f>
         <v>  </v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="str">
+      <c r="A30" s="3" t="str">
         <f aca="false">people!A30&amp;" "&amp;people!B30&amp;" "&amp;people!C30</f>
         <v>  </v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="str">
+      <c r="A31" s="3" t="str">
         <f aca="false">people!A31&amp;" "&amp;people!B31&amp;" "&amp;people!C31</f>
         <v>  </v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="str">
+      <c r="A32" s="3" t="str">
         <f aca="false">people!A32&amp;" "&amp;people!B32&amp;" "&amp;people!C32</f>
         <v>  </v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8" t="str">
+      <c r="A33" s="3" t="str">
         <f aca="false">people!A33&amp;" "&amp;people!B33&amp;" "&amp;people!C33</f>
         <v>  </v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8" t="str">
+      <c r="A34" s="3" t="str">
         <f aca="false">people!A34&amp;" "&amp;people!B34&amp;" "&amp;people!C34</f>
         <v>  </v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="8" t="str">
+      <c r="A35" s="3" t="str">
         <f aca="false">people!A35&amp;" "&amp;people!B35&amp;" "&amp;people!C35</f>
         <v>  </v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8" t="str">
+      <c r="A36" s="3" t="str">
         <f aca="false">people!A36&amp;" "&amp;people!B36&amp;" "&amp;people!C36</f>
         <v>  </v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8" t="str">
+      <c r="A37" s="3" t="str">
         <f aca="false">people!A37&amp;" "&amp;people!B37&amp;" "&amp;people!C37</f>
         <v>  </v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="8" t="str">
+      <c r="A38" s="3" t="str">
         <f aca="false">people!A38&amp;" "&amp;people!B38&amp;" "&amp;people!C38</f>
         <v>  </v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="8" t="str">
+      <c r="A39" s="3" t="str">
         <f aca="false">people!A39&amp;" "&amp;people!B39&amp;" "&amp;people!C39</f>
         <v>  </v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8" t="str">
+      <c r="A40" s="3" t="str">
         <f aca="false">people!A40&amp;" "&amp;people!B40&amp;" "&amp;people!C40</f>
         <v>  </v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8" t="str">
+      <c r="A41" s="3" t="str">
         <f aca="false">people!A41&amp;" "&amp;people!B41&amp;" "&amp;people!C41</f>
         <v>  </v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8" t="str">
+      <c r="A42" s="3" t="str">
         <f aca="false">people!A42&amp;" "&amp;people!B42&amp;" "&amp;people!C42</f>
         <v>  </v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8" t="str">
+      <c r="A43" s="3" t="str">
         <f aca="false">people!A43&amp;" "&amp;people!B43&amp;" "&amp;people!C43</f>
         <v>  </v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="8" t="str">
+      <c r="A44" s="3" t="str">
         <f aca="false">people!A44&amp;" "&amp;people!B44&amp;" "&amp;people!C44</f>
         <v>  </v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="8" t="str">
+      <c r="A45" s="3" t="str">
         <f aca="false">people!A45&amp;" "&amp;people!B45&amp;" "&amp;people!C45</f>
         <v>  </v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8" t="str">
+      <c r="A46" s="3" t="str">
         <f aca="false">people!A46&amp;" "&amp;people!B46&amp;" "&amp;people!C46</f>
         <v>  </v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8" t="str">
+      <c r="A47" s="3" t="str">
         <f aca="false">people!A47&amp;" "&amp;people!B47&amp;" "&amp;people!C47</f>
         <v>  </v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="8" t="str">
+      <c r="A48" s="3" t="str">
         <f aca="false">people!A48&amp;" "&amp;people!B48&amp;" "&amp;people!C48</f>
         <v>  </v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8" t="str">
+      <c r="A49" s="3" t="str">
         <f aca="false">people!A49&amp;" "&amp;people!B49&amp;" "&amp;people!C49</f>
         <v>  </v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="8" t="str">
+      <c r="A50" s="3" t="str">
         <f aca="false">people!A50&amp;" "&amp;people!B50&amp;" "&amp;people!C50</f>
         <v>  </v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="str">
+      <c r="A51" s="3" t="str">
         <f aca="false">people!A51&amp;" "&amp;people!B51&amp;" "&amp;people!C51</f>
         <v>  </v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="8" t="str">
+      <c r="A52" s="3" t="str">
         <f aca="false">people!A52&amp;" "&amp;people!B52&amp;" "&amp;people!C52</f>
         <v>  </v>
       </c>

</xml_diff>